<commit_message>
Scenarios to write search record to excel
</commit_message>
<xml_diff>
--- a/GoogleSearchResult.xlsx
+++ b/GoogleSearchResult.xlsx
@@ -1,37 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -50,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -330,13 +385,202 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Records</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Java Tutorial</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Java.Oracle.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Java Downloads</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>What is Java? - Java Programming Language Explained - AWS</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Increment and Decrement Operators in Java - Dummies.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>How to Program in Java: 3 Steps (with Pictures) - wikiHow</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>What Is Java? - IBM</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>What Is The Future Of Java Developers - SkillVertex</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Is Java Difficult to Learn? Explore the Challenges! - Simplilearn.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>What is Java Used For in 2023? The Java Programming Language and ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>What is the full form of Java? - Tutorialspoint</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>What is Java?—Beginner's Guide to Java | Microsoft Azure</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>What Is Java? - IBM</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Java Tutorial</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Java (programming language)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Java Tutorial | Learn Java Programming</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Welcome to Python.org</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Python Tutorial</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Selenium</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Selenium Testing: Detailed Guide</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>SeleniumHQ/selenium: A browser automation framework ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Selenium Webdriver Tutorial in Java with Examples | BrowserStack</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Selenium Test Automation: Choosing the Right Programming Language ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Selenium Testing: Detailed Guide</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>SeleniumHQ/selenium: A browser automation framework ...</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>